<commit_message>
updated sample sheets with default timings
</commit_message>
<xml_diff>
--- a/samplesheets/jldc.xlsx
+++ b/samplesheets/jldc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\session2\samplesheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\downloads\SHEETS-20240528T041642Z-001\SHEETS\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D43E14-5EDB-42ED-86CA-3C796E365CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6A6BCC6-7ABF-4722-8C9B-EE7C5B035B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14955" yWindow="3135" windowWidth="13845" windowHeight="9885" xr2:uid="{7033BC65-021F-4BF8-AC31-7CE247724AC8}"/>
+    <workbookView xWindow="7110" yWindow="5610" windowWidth="13845" windowHeight="9885" xr2:uid="{7033BC65-021F-4BF8-AC31-7CE247724AC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
   <si>
     <t>TIME (HRS)</t>
   </si>
@@ -33,7 +33,295 @@
     <t>Date</t>
   </si>
   <si>
-    <t>POWER GENERATION</t>
+    <t>00:00 - 00:15</t>
+  </si>
+  <si>
+    <t>00:15 - 00:30</t>
+  </si>
+  <si>
+    <t>00:30 - 00:45</t>
+  </si>
+  <si>
+    <t>00:45 - 01:00</t>
+  </si>
+  <si>
+    <t>01:00 - 01:15</t>
+  </si>
+  <si>
+    <t>01:00 - 01:16</t>
+  </si>
+  <si>
+    <t>01:30 - 01:45</t>
+  </si>
+  <si>
+    <t>01:45 - 02:00</t>
+  </si>
+  <si>
+    <t>02:00 - 02:15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Power Generation </t>
+  </si>
+  <si>
+    <t>02:15 - 02:30</t>
+  </si>
+  <si>
+    <t>02:30 - 02:45</t>
+  </si>
+  <si>
+    <t>02:45 - 03:00</t>
+  </si>
+  <si>
+    <t>03:00 - 03:15</t>
+  </si>
+  <si>
+    <t>03:15 - 03:30</t>
+  </si>
+  <si>
+    <t>03:30 - 03:45</t>
+  </si>
+  <si>
+    <t>03:45 - 04:00</t>
+  </si>
+  <si>
+    <t>04:00 - 04:15</t>
+  </si>
+  <si>
+    <t>04:15 - 04:30</t>
+  </si>
+  <si>
+    <t>04:30 - 04:45</t>
+  </si>
+  <si>
+    <t>04:45 - 05:00</t>
+  </si>
+  <si>
+    <t>05:00 - 05:15</t>
+  </si>
+  <si>
+    <t>05:15 - 05:30</t>
+  </si>
+  <si>
+    <t>05:30 - 05:45</t>
+  </si>
+  <si>
+    <t>05:45 - 06:00</t>
+  </si>
+  <si>
+    <t>06:00 - 06:15</t>
+  </si>
+  <si>
+    <t>06:15 - 06:30</t>
+  </si>
+  <si>
+    <t>06:30 - 06:45</t>
+  </si>
+  <si>
+    <t>06:45 - 07:00</t>
+  </si>
+  <si>
+    <t>07:00 - 07:15</t>
+  </si>
+  <si>
+    <t>07:15 - 07:30</t>
+  </si>
+  <si>
+    <t>07:30 - 07:45</t>
+  </si>
+  <si>
+    <t>07:45 - 08:00</t>
+  </si>
+  <si>
+    <t>08:00 - 08:15</t>
+  </si>
+  <si>
+    <t>08:15 - 08:30</t>
+  </si>
+  <si>
+    <t>08:30 - 08:45</t>
+  </si>
+  <si>
+    <t>08:45 - 09:00</t>
+  </si>
+  <si>
+    <t>09:00 - 09:15</t>
+  </si>
+  <si>
+    <t>09:15 - 09:30</t>
+  </si>
+  <si>
+    <t>09:30 - 09:45</t>
+  </si>
+  <si>
+    <t>09:45 - 10:00</t>
+  </si>
+  <si>
+    <t>10:00 - 10:15</t>
+  </si>
+  <si>
+    <t>10:15 - 10:30</t>
+  </si>
+  <si>
+    <t>10:30 - 10:45</t>
+  </si>
+  <si>
+    <t>10:45 - 11:00</t>
+  </si>
+  <si>
+    <t>11:00 - 11:15</t>
+  </si>
+  <si>
+    <t>11:15 - 11:30</t>
+  </si>
+  <si>
+    <t>11:30 - 11:45</t>
+  </si>
+  <si>
+    <t>11:45 - 12:00</t>
+  </si>
+  <si>
+    <t>12:00 - 12:15</t>
+  </si>
+  <si>
+    <t>12:15 - 12:30</t>
+  </si>
+  <si>
+    <t>12:30 - 12:45</t>
+  </si>
+  <si>
+    <t>12:45 - 13:00</t>
+  </si>
+  <si>
+    <t>13:00 - 13:15</t>
+  </si>
+  <si>
+    <t>13:15 - 13:30</t>
+  </si>
+  <si>
+    <t>13:30 - 13:45</t>
+  </si>
+  <si>
+    <t>13:45 - 14:00</t>
+  </si>
+  <si>
+    <t>14:00 - 14:15</t>
+  </si>
+  <si>
+    <t>14:15 - 14:30</t>
+  </si>
+  <si>
+    <t>14:30 - 14:45</t>
+  </si>
+  <si>
+    <t>14:45 - 15:00</t>
+  </si>
+  <si>
+    <t>15:00 - 15:15</t>
+  </si>
+  <si>
+    <t>15:15 - 15:30</t>
+  </si>
+  <si>
+    <t>15:30 - 15:45</t>
+  </si>
+  <si>
+    <t>15:45 - 16:00</t>
+  </si>
+  <si>
+    <t>16:00 - 16:15</t>
+  </si>
+  <si>
+    <t>16:15 - 16:30</t>
+  </si>
+  <si>
+    <t>16:30 - 16:45</t>
+  </si>
+  <si>
+    <t>16:45 - 17:00</t>
+  </si>
+  <si>
+    <t>17:00 - 17:15</t>
+  </si>
+  <si>
+    <t>17:15 - 17:30</t>
+  </si>
+  <si>
+    <t>17:30 - 17:45</t>
+  </si>
+  <si>
+    <t>17:45 - 18:00</t>
+  </si>
+  <si>
+    <t>18:00 - 18:15</t>
+  </si>
+  <si>
+    <t>18:15 - 18:30</t>
+  </si>
+  <si>
+    <t>18:30 - 18:45</t>
+  </si>
+  <si>
+    <t>18:45 - 19:00</t>
+  </si>
+  <si>
+    <t>19:00 - 19:15</t>
+  </si>
+  <si>
+    <t>19:15 - 19:30</t>
+  </si>
+  <si>
+    <t>19:30 - 19:45</t>
+  </si>
+  <si>
+    <t>19:45 - 20:00</t>
+  </si>
+  <si>
+    <t>20:00 - 20:15</t>
+  </si>
+  <si>
+    <t>20:15 - 20:30</t>
+  </si>
+  <si>
+    <t>20:30 - 20:45</t>
+  </si>
+  <si>
+    <t>20:45 - 21:00</t>
+  </si>
+  <si>
+    <t>21:00 - 21:15</t>
+  </si>
+  <si>
+    <t>21:15 - 21:30</t>
+  </si>
+  <si>
+    <t>21:30 - 21:45</t>
+  </si>
+  <si>
+    <t>21:45 - 22:00</t>
+  </si>
+  <si>
+    <t>22:00 - 22:15</t>
+  </si>
+  <si>
+    <t>22:15 - 22:30</t>
+  </si>
+  <si>
+    <t>22:30 - 22:45</t>
+  </si>
+  <si>
+    <t>22:45 - 23:00</t>
+  </si>
+  <si>
+    <t>23:00 - 23:15</t>
+  </si>
+  <si>
+    <t>23:15 - 23:30</t>
+  </si>
+  <si>
+    <t>23:30 - 23:45</t>
+  </si>
+  <si>
+    <t>23:45 - 24:00</t>
   </si>
 </sst>
 </file>
@@ -43,7 +331,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d\-mmm\-yyyy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,17 +344,27 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -107,8 +405,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -118,15 +417,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{2AFE6465-41FE-44A3-830E-FF42A1C3C0AA}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -438,10 +738,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C183429-DACA-446F-A911-DB6FA677D8D1}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection sqref="A1:C97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,53 +757,872 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="4"/>
+      <c r="B2" s="4">
+        <v>45325</v>
+      </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4"/>
+      <c r="A3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="4">
+        <v>45325</v>
+      </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
+      <c r="A4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="4">
+        <v>45325</v>
+      </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4"/>
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4">
+        <v>45325</v>
+      </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="4">
+        <v>45325</v>
+      </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="4">
+        <v>45325</v>
+      </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="4">
+        <v>45325</v>
+      </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
+      <c r="A9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4">
+        <v>45325</v>
+      </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="4"/>
+      <c r="A10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="4">
+        <v>45325</v>
+      </c>
       <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C20" s="2"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C22" s="2"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C23" s="2"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C25" s="2"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C26" s="2"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C31" s="2"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B32" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C32" s="2"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C33" s="2"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C34" s="2"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C35" s="2"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C36" s="2"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C39" s="2"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C40" s="2"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C41" s="2"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C42" s="2"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C43" s="2"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B44" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C44" s="2"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C45" s="2"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C46" s="2"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B47" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C47" s="2"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C48" s="2"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C49" s="2"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C50" s="2"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C51" s="2"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C52" s="2"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B53" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C53" s="2"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C54" s="2"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B55" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C55" s="2"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C56" s="2"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C57" s="2"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B58" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C58" s="2"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B59" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C59" s="2"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B60" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C60" s="2"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B61" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C61" s="2"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C62" s="2"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B63" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C63" s="2"/>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B64" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C64" s="2"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B65" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C65" s="2"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B66" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C66" s="2"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B67" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C67" s="2"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B68" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C68" s="2"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B69" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C69" s="2"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B70" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C70" s="2"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B71" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C71" s="2"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B72" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C72" s="2"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B73" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C73" s="2"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B74" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C74" s="2"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B75" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C75" s="2"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B76" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C76" s="2"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B77" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C77" s="2"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B78" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C78" s="2"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B79" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C79" s="2"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B80" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C80" s="2"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B81" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C81" s="2"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B82" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C82" s="2"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B83" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C83" s="2"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B84" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C84" s="2"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B85" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C85" s="2"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B86" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C86" s="2"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B87" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C87" s="2"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B88" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C88" s="2"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B89" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C89" s="2"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B90" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C90" s="2"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B91" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C91" s="2"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B92" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C92" s="2"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B93" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C93" s="2"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B94" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C94" s="2"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B95" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C95" s="2"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B96" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C96" s="2"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B97" s="4">
+        <v>45325</v>
+      </c>
+      <c r="C97" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>